<commit_message>
Release notes: Removed No longer used content (SVNClient, ThinClient, updateTest). Updated Packets.xlsx Changed Multi-comment Format rule. Updated server revision in server. In progress: Rewriting sending and receiving of new pakcets. Server can receive a few new packets and client now send new login and movement packets.
NOTE:Client is not compatible with online servers in current state!!
</commit_message>
<xml_diff>
--- a/RN and Misc/Packets.xlsx
+++ b/RN and Misc/Packets.xlsx
@@ -15,8 +15,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Rémy Baratté</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rémy Baratté:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In-game ID's are regular numbers. IE: 0A = 10
+Read the row number - 1.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="617">
   <si>
     <t>Packet ID</t>
   </si>
@@ -1770,9 +1805,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Unused</t>
-  </si>
-  <si>
     <t>Account Server Offline</t>
   </si>
   <si>
@@ -1858,19 +1890,44 @@
   </si>
   <si>
     <t>Email Address Already Registered</t>
+  </si>
+  <si>
+    <t>Unused?</t>
+  </si>
+  <si>
+    <t>Tested</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2205,25 +2262,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2239,8 +2296,11 @@
       <c r="E1" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2253,8 +2313,11 @@
       <c r="E2" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2267,8 +2330,11 @@
       <c r="E3" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2281,8 +2347,11 @@
       <c r="E4" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="2" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -2295,8 +2364,11 @@
       <c r="E5" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -2307,13 +2379,16 @@
         <v>276</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>584</v>
+        <v>613</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -2324,13 +2399,16 @@
         <v>275</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>584</v>
+        <v>613</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -2341,13 +2419,16 @@
         <v>277</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>584</v>
+        <v>613</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -2358,13 +2439,16 @@
         <v>278</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>584</v>
+        <v>613</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -2378,8 +2462,11 @@
       <c r="E10" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -2392,8 +2479,11 @@
       <c r="E11" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -2406,8 +2496,11 @@
       <c r="E12" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -2420,8 +2513,11 @@
       <c r="E13" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -2434,8 +2530,11 @@
       <c r="E14" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
@@ -2449,7 +2548,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
@@ -3053,6 +3152,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3061,10 +3161,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:F116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3075,7 +3175,7 @@
     <col min="5" max="5" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3091,8 +3191,11 @@
       <c r="E1" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -3106,7 +3209,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -3120,7 +3223,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -3134,7 +3237,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -3148,7 +3251,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -3162,7 +3265,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -3176,7 +3279,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -3190,7 +3293,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -3204,7 +3307,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -3218,7 +3321,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
@@ -3232,7 +3335,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
@@ -3246,7 +3349,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
@@ -3260,7 +3363,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
@@ -3274,7 +3377,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>24</v>
       </c>
@@ -3288,7 +3391,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>25</v>
       </c>
@@ -4083,7 +4186,7 @@
         <v>562</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>584</v>
+        <v>613</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>151</v>
@@ -4100,7 +4203,7 @@
         <v>563</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>584</v>
+        <v>613</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>151</v>
@@ -4117,7 +4220,7 @@
         <v>564</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>584</v>
+        <v>613</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>151</v>
@@ -4134,7 +4237,7 @@
         <v>565</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>584</v>
+        <v>613</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>151</v>
@@ -4386,7 +4489,7 @@
         <v>233</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>151</v>
@@ -4400,7 +4503,7 @@
         <v>234</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>151</v>
@@ -4414,7 +4517,7 @@
         <v>235</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>151</v>
@@ -4428,7 +4531,7 @@
         <v>236</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>151</v>
@@ -4442,7 +4545,7 @@
         <v>237</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>151</v>
@@ -4456,7 +4559,7 @@
         <v>238</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>151</v>
@@ -4470,7 +4573,7 @@
         <v>239</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>151</v>
@@ -4481,10 +4584,10 @@
         <v>255</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>151</v>
@@ -4495,10 +4598,10 @@
         <v>256</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>151</v>
@@ -4512,7 +4615,7 @@
         <v>240</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>151</v>
@@ -4526,7 +4629,7 @@
         <v>241</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>151</v>
@@ -4540,7 +4643,7 @@
         <v>242</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>151</v>
@@ -4554,7 +4657,7 @@
         <v>243</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>151</v>
@@ -4568,7 +4671,7 @@
         <v>244</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>151</v>
@@ -4610,7 +4713,7 @@
         <v>113</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>151</v>
@@ -4624,7 +4727,7 @@
         <v>245</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>151</v>
@@ -4638,7 +4741,7 @@
         <v>180</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>151</v>
@@ -4652,7 +4755,7 @@
         <v>181</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>151</v>
@@ -4663,10 +4766,10 @@
         <v>268</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>151</v>
@@ -4677,10 +4780,10 @@
         <v>270</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>151</v>
@@ -4688,13 +4791,13 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>151</v>
@@ -4702,13 +4805,13 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>151</v>
@@ -4727,7 +4830,7 @@
   </sheetPr>
   <dimension ref="A1:A173"/>
   <sheetViews>
-    <sheetView topLeftCell="A146" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Completed Receiving end of new packets in the Server (Currently Untested). Cleaned up some code.
</commit_message>
<xml_diff>
--- a/RN and Misc/Packets.xlsx
+++ b/RN and Misc/Packets.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="625">
   <si>
     <t>Packet ID</t>
   </si>
@@ -434,9 +434,6 @@
     <t>Mk</t>
   </si>
   <si>
-    <t>Mw</t>
-  </si>
-  <si>
     <t>Mwn</t>
   </si>
   <si>
@@ -962,9 +959,6 @@
     <t>Kick Player</t>
   </si>
   <si>
-    <t>Change Weather on Map</t>
-  </si>
-  <si>
     <t>Normal Weather</t>
   </si>
   <si>
@@ -1013,9 +1007,6 @@
     <t>Make Trade Offer</t>
   </si>
   <si>
-    <t>Ready for Trade</t>
-  </si>
-  <si>
     <t>Cancel Trade</t>
   </si>
   <si>
@@ -1902,6 +1893,39 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Buy Sprite</t>
+  </si>
+  <si>
+    <t>Mc</t>
+  </si>
+  <si>
+    <t>Player Count</t>
+  </si>
+  <si>
+    <t>Fo</t>
+  </si>
+  <si>
+    <t>Check Friend Online Status</t>
+  </si>
+  <si>
+    <t>Give Item</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Trade Offer Accepted</t>
+  </si>
+  <si>
+    <t>Cw</t>
+  </si>
+  <si>
+    <t>World Chat</t>
   </si>
 </sst>
 </file>
@@ -2266,10 +2290,10 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2277,6 +2301,7 @@
     <col min="1" max="1" width="9.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2288,16 +2313,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2308,13 +2333,14 @@
         <v>93</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>273</v>
-      </c>
+        <v>272</v>
+      </c>
+      <c r="D2" s="1"/>
       <c r="E2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2325,13 +2351,14 @@
         <v>94</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>272</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2342,13 +2369,16 @@
         <v>95</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>610</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2359,13 +2389,14 @@
         <v>96</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>274</v>
-      </c>
+        <v>273</v>
+      </c>
+      <c r="D5" s="1"/>
       <c r="E5" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2376,16 +2407,14 @@
         <v>97</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>613</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2396,16 +2425,14 @@
         <v>98</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>613</v>
-      </c>
+        <v>274</v>
+      </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2416,16 +2443,14 @@
         <v>99</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>613</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2436,16 +2461,14 @@
         <v>100</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>613</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2456,14 +2479,14 @@
         <v>101</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2474,13 +2497,14 @@
         <v>102</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>280</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="D11" s="1"/>
       <c r="E11" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2491,13 +2515,14 @@
         <v>103</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>281</v>
-      </c>
+        <v>280</v>
+      </c>
+      <c r="D12" s="1"/>
       <c r="E12" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2508,13 +2533,14 @@
         <v>104</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>282</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="D13" s="1"/>
       <c r="E13" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2525,13 +2551,14 @@
         <v>105</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>283</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="D14" s="1"/>
       <c r="E14" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2539,13 +2566,17 @@
         <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>106</v>
+        <v>614</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>284</v>
-      </c>
+        <v>615</v>
+      </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="2" t="s">
         <v>31</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>613</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2553,601 +2584,845 @@
         <v>25</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>285</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="D16" s="1"/>
       <c r="E16" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>286</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="D17" s="1"/>
       <c r="E17" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>287</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="D18" s="1"/>
       <c r="E18" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>288</v>
-      </c>
+        <v>286</v>
+      </c>
+      <c r="D19" s="1"/>
       <c r="E19" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>289</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="D20" s="1"/>
       <c r="E20" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>290</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="D21" s="1"/>
       <c r="E21" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>291</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="D22" s="1"/>
       <c r="E22" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>292</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="D23" s="1"/>
       <c r="E23" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>293</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="D24" s="1"/>
       <c r="E24" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>517</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="D25" s="1"/>
       <c r="E25" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>294</v>
-      </c>
+        <v>514</v>
+      </c>
+      <c r="D26" s="1"/>
       <c r="E26" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>295</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="D27" s="1"/>
       <c r="E27" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>119</v>
+        <v>616</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>296</v>
-      </c>
+        <v>617</v>
+      </c>
+      <c r="D28" s="1"/>
       <c r="E28" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>297</v>
-      </c>
+        <v>294</v>
+      </c>
+      <c r="D29" s="1"/>
       <c r="E29" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>298</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="D30" s="1"/>
       <c r="E30" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>299</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="D31" s="1"/>
       <c r="E31" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>300</v>
-      </c>
+        <v>297</v>
+      </c>
+      <c r="D32" s="1"/>
       <c r="E32" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>301</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="D33" s="1"/>
       <c r="E33" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>302</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="D34" s="1"/>
       <c r="E34" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>303</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="D35" s="1"/>
       <c r="E35" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>304</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="D36" s="1"/>
       <c r="E36" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>305</v>
-      </c>
+        <v>302</v>
+      </c>
+      <c r="D37" s="1"/>
       <c r="E37" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>306</v>
-      </c>
+        <v>303</v>
+      </c>
+      <c r="D38" s="1"/>
       <c r="E38" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>307</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="D39" s="1"/>
       <c r="E39" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>309</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="D40" s="1"/>
       <c r="E40" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>212</v>
+        <v>131</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>308</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="D41" s="1"/>
       <c r="E41" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>133</v>
+        <v>211</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>310</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="D42" s="1"/>
       <c r="E42" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>311</v>
-      </c>
+        <v>308</v>
+      </c>
+      <c r="D43" s="1"/>
       <c r="E43" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>312</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="D44" s="1"/>
       <c r="E44" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>313</v>
-      </c>
+        <v>310</v>
+      </c>
+      <c r="D45" s="1"/>
       <c r="E45" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>314</v>
-      </c>
+        <v>311</v>
+      </c>
+      <c r="D46" s="1"/>
       <c r="E46" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>316</v>
-      </c>
+        <v>312</v>
+      </c>
+      <c r="D47" s="1"/>
       <c r="E47" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>315</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="D48" s="1"/>
       <c r="E48" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>317</v>
-      </c>
+        <v>313</v>
+      </c>
+      <c r="D49" s="1"/>
       <c r="E49" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>141</v>
+        <v>618</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>318</v>
-      </c>
+        <v>619</v>
+      </c>
+      <c r="D50" s="1"/>
       <c r="E50" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>319</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="D51" s="1"/>
       <c r="E51" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>143</v>
+        <v>621</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>320</v>
-      </c>
+        <v>620</v>
+      </c>
+      <c r="D52" s="1"/>
       <c r="E52" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>322</v>
-      </c>
+        <v>316</v>
+      </c>
+      <c r="D53" s="1"/>
       <c r="E53" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>321</v>
-      </c>
+        <v>317</v>
+      </c>
+      <c r="D54" s="1"/>
       <c r="E54" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>323</v>
-      </c>
+        <v>622</v>
+      </c>
+      <c r="D55" s="1"/>
       <c r="E55" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>324</v>
-      </c>
+        <v>319</v>
+      </c>
+      <c r="D56" s="1"/>
       <c r="E56" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>325</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="D57" s="1"/>
       <c r="E57" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>149</v>
+        <v>623</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>326</v>
-      </c>
+        <v>624</v>
+      </c>
+      <c r="D58" s="1"/>
       <c r="E58" s="2" t="s">
         <v>31</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D59" s="1"/>
+      <c r="E59" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D60" s="1"/>
+      <c r="E60" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D62" s="1"/>
+      <c r="E62" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>613</v>
       </c>
     </row>
   </sheetData>
@@ -3164,7 +3439,7 @@
   <dimension ref="A1:F116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3183,16 +3458,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3203,10 +3478,10 @@
         <v>100</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3214,13 +3489,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3228,13 +3503,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3242,13 +3517,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3256,13 +3531,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3270,13 +3545,13 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3284,13 +3559,13 @@
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3298,13 +3573,13 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3315,10 +3590,10 @@
         <v>105</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3326,13 +3601,13 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3340,13 +3615,13 @@
         <v>21</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3357,10 +3632,10 @@
         <v>108</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3368,13 +3643,13 @@
         <v>23</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3382,13 +3657,13 @@
         <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -3399,10 +3674,10 @@
         <v>106</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3413,10 +3688,10 @@
         <v>107</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3424,13 +3699,13 @@
         <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3438,13 +3713,13 @@
         <v>13</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3452,13 +3727,13 @@
         <v>14</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3466,13 +3741,13 @@
         <v>15</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3480,13 +3755,13 @@
         <v>16</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3494,13 +3769,13 @@
         <v>17</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3508,13 +3783,13 @@
         <v>18</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3522,13 +3797,13 @@
         <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3536,13 +3811,13 @@
         <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3550,13 +3825,13 @@
         <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -3564,13 +3839,13 @@
         <v>63</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3578,13 +3853,13 @@
         <v>64</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3592,13 +3867,13 @@
         <v>65</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3606,13 +3881,13 @@
         <v>66</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -3620,13 +3895,13 @@
         <v>67</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3634,13 +3909,13 @@
         <v>28</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3648,13 +3923,13 @@
         <v>29</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3662,13 +3937,13 @@
         <v>32</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3676,13 +3951,13 @@
         <v>33</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3690,13 +3965,13 @@
         <v>34</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3704,13 +3979,13 @@
         <v>35</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3718,13 +3993,13 @@
         <v>36</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3732,13 +4007,13 @@
         <v>37</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -3746,13 +4021,13 @@
         <v>38</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -3760,13 +4035,13 @@
         <v>39</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3774,13 +4049,13 @@
         <v>40</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3788,13 +4063,13 @@
         <v>41</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3802,13 +4077,13 @@
         <v>42</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -3816,13 +4091,13 @@
         <v>43</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3830,13 +4105,13 @@
         <v>44</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3844,13 +4119,13 @@
         <v>45</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3858,13 +4133,13 @@
         <v>46</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3872,13 +4147,13 @@
         <v>47</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3886,13 +4161,13 @@
         <v>48</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -3900,13 +4175,13 @@
         <v>49</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3914,13 +4189,13 @@
         <v>50</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -3928,13 +4203,13 @@
         <v>51</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3942,13 +4217,13 @@
         <v>52</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -3956,13 +4231,13 @@
         <v>53</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3970,13 +4245,13 @@
         <v>54</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3984,13 +4259,13 @@
         <v>55</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -3998,13 +4273,13 @@
         <v>56</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -4012,13 +4287,13 @@
         <v>57</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -4026,13 +4301,13 @@
         <v>58</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -4040,13 +4315,13 @@
         <v>59</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -4054,13 +4329,13 @@
         <v>60</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -4068,13 +4343,13 @@
         <v>61</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -4082,13 +4357,13 @@
         <v>62</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -4096,13 +4371,13 @@
         <v>68</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -4110,13 +4385,13 @@
         <v>69</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -4124,13 +4399,13 @@
         <v>70</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -4138,13 +4413,13 @@
         <v>71</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -4152,13 +4427,13 @@
         <v>72</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -4166,13 +4441,13 @@
         <v>73</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -4180,16 +4455,16 @@
         <v>74</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -4197,16 +4472,16 @@
         <v>75</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -4214,16 +4489,16 @@
         <v>76</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -4231,16 +4506,16 @@
         <v>77</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -4248,13 +4523,13 @@
         <v>78</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -4265,10 +4540,10 @@
         <v>97</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -4279,10 +4554,10 @@
         <v>121</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -4290,13 +4565,13 @@
         <v>81</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -4304,13 +4579,13 @@
         <v>82</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -4318,13 +4593,13 @@
         <v>83</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -4332,13 +4607,13 @@
         <v>84</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -4346,13 +4621,13 @@
         <v>85</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -4360,13 +4635,13 @@
         <v>86</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -4374,13 +4649,13 @@
         <v>87</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -4388,13 +4663,13 @@
         <v>88</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -4402,13 +4677,13 @@
         <v>89</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -4416,13 +4691,13 @@
         <v>90</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -4430,13 +4705,13 @@
         <v>91</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -4444,377 +4719,377 @@
         <v>92</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>110</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>113</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B113" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="C113" s="2" t="s">
         <v>608</v>
       </c>
-      <c r="C113" s="2" t="s">
-        <v>611</v>
-      </c>
       <c r="E113" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -4841,862 +5116,862 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Client now sends new packets to Server.
Renamed current server code to Server hopefully stopping SourceForge and/or Windows chokes on Path limit.
Rared original server code to RN and Misc Folder.
All packets that I was able to test have been tested and documented.
Overall code cleanup in some places.
</commit_message>
<xml_diff>
--- a/RN and Misc/Packets.xlsx
+++ b/RN and Misc/Packets.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="636">
   <si>
     <t>Packet ID</t>
   </si>
@@ -356,18 +356,6 @@
     <t>R</t>
   </si>
   <si>
-    <t>pm</t>
-  </si>
-  <si>
-    <t>pM</t>
-  </si>
-  <si>
-    <t>pe0</t>
-  </si>
-  <si>
-    <t>pe1</t>
-  </si>
-  <si>
     <t>s</t>
   </si>
   <si>
@@ -1001,9 +989,6 @@
     <t>Use Item</t>
   </si>
   <si>
-    <t>Drop Item</t>
-  </si>
-  <si>
     <t>Make Trade Offer</t>
   </si>
   <si>
@@ -1926,6 +1911,54 @@
   </si>
   <si>
     <t>World Chat</t>
+  </si>
+  <si>
+    <t>Snow or Hail</t>
+  </si>
+  <si>
+    <t>Muf Sent</t>
+  </si>
+  <si>
+    <t>Drop (Destroy) Item</t>
+  </si>
+  <si>
+    <t>Pe0</t>
+  </si>
+  <si>
+    <t>Pe1</t>
+  </si>
+  <si>
+    <t>Duplicate?</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>Use Bag Hotbar</t>
+  </si>
+  <si>
+    <t>Implement</t>
+  </si>
+  <si>
+    <t>Normal or Sunny Weather</t>
+  </si>
+  <si>
+    <t>Hail/Rain</t>
+  </si>
+  <si>
+    <t>Random :3</t>
+  </si>
+  <si>
+    <t>Sunny</t>
+  </si>
+  <si>
+    <t>GUI doesn't like</t>
+  </si>
+  <si>
+    <t>Bugged Locally</t>
   </si>
 </sst>
 </file>
@@ -2290,10 +2323,10 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2301,7 +2334,7 @@
     <col min="1" max="1" width="9.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2313,16 +2346,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2333,14 +2366,14 @@
         <v>93</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2351,14 +2384,14 @@
         <v>94</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2369,16 +2402,16 @@
         <v>95</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2389,14 +2422,14 @@
         <v>96</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2407,14 +2440,14 @@
         <v>97</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2425,14 +2458,14 @@
         <v>98</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2443,14 +2476,14 @@
         <v>99</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2461,14 +2494,14 @@
         <v>100</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2476,17 +2509,17 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>101</v>
+        <v>184</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2494,17 +2527,17 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>102</v>
+        <v>185</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2512,17 +2545,17 @@
         <v>21</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>103</v>
+        <v>623</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2530,17 +2563,17 @@
         <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>104</v>
+        <v>624</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2548,17 +2581,17 @@
         <v>23</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2566,17 +2599,17 @@
         <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2584,17 +2617,17 @@
         <v>25</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2602,17 +2635,17 @@
         <v>11</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2620,17 +2653,17 @@
         <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2638,17 +2671,17 @@
         <v>13</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2656,17 +2689,17 @@
         <v>14</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2674,17 +2707,17 @@
         <v>15</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2692,17 +2725,17 @@
         <v>16</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2710,17 +2743,17 @@
         <v>17</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2728,17 +2761,17 @@
         <v>18</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2746,17 +2779,17 @@
         <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2764,17 +2797,17 @@
         <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2782,17 +2815,17 @@
         <v>27</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2800,17 +2833,17 @@
         <v>63</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2818,17 +2851,19 @@
         <v>64</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="D29" s="1"/>
+        <v>290</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>625</v>
+      </c>
       <c r="E29" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2836,17 +2871,17 @@
         <v>65</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2854,17 +2889,17 @@
         <v>66</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2872,17 +2907,19 @@
         <v>67</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D32" s="1"/>
+        <v>293</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>629</v>
+      </c>
       <c r="E32" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2890,17 +2927,17 @@
         <v>28</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2908,17 +2945,17 @@
         <v>29</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2926,17 +2963,17 @@
         <v>32</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2944,17 +2981,17 @@
         <v>33</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2962,17 +2999,19 @@
         <v>34</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="D37" s="1"/>
+        <v>630</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>633</v>
+      </c>
       <c r="E37" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2980,17 +3019,19 @@
         <v>35</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="D38" s="1"/>
+        <v>299</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>299</v>
+      </c>
       <c r="E38" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2998,17 +3039,19 @@
         <v>36</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="D39" s="1"/>
+        <v>620</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>300</v>
+      </c>
       <c r="E39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -3016,17 +3059,19 @@
         <v>37</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="D40" s="1"/>
+        <v>301</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>621</v>
+      </c>
       <c r="E40" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -3034,17 +3079,19 @@
         <v>38</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="D41" s="1"/>
+        <v>303</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>631</v>
+      </c>
       <c r="E41" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -3052,17 +3099,19 @@
         <v>39</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="D42" s="1"/>
+        <v>302</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>632</v>
+      </c>
       <c r="E42" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -3070,17 +3119,19 @@
         <v>40</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="D43" s="1"/>
+        <v>304</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>634</v>
+      </c>
       <c r="E43" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -3088,17 +3139,19 @@
         <v>41</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="D44" s="1"/>
+        <v>305</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>625</v>
+      </c>
       <c r="E44" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -3106,17 +3159,17 @@
         <v>42</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -3124,17 +3177,17 @@
         <v>43</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -3142,17 +3195,17 @@
         <v>44</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -3160,17 +3213,17 @@
         <v>45</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -3178,17 +3231,17 @@
         <v>46</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -3196,17 +3249,17 @@
         <v>47</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -3214,17 +3267,17 @@
         <v>48</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -3232,17 +3285,17 @@
         <v>49</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -3250,17 +3303,17 @@
         <v>50</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>316</v>
+        <v>622</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -3268,17 +3321,17 @@
         <v>51</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -3286,17 +3339,17 @@
         <v>52</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -3304,17 +3357,17 @@
         <v>53</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -3322,17 +3375,17 @@
         <v>54</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -3340,17 +3393,17 @@
         <v>55</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -3358,17 +3411,19 @@
         <v>56</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="D59" s="1"/>
+        <v>315</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>635</v>
+      </c>
       <c r="E59" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -3376,17 +3431,17 @@
         <v>57</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -3394,17 +3449,17 @@
         <v>58</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -3412,17 +3467,37 @@
         <v>59</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>607</v>
       </c>
     </row>
   </sheetData>
@@ -3439,7 +3514,7 @@
   <dimension ref="A1:F116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3458,16 +3533,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3478,10 +3553,10 @@
         <v>100</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3489,13 +3564,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3503,13 +3578,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3517,13 +3592,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3531,13 +3606,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3545,13 +3620,13 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3559,13 +3634,13 @@
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3573,13 +3648,13 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3587,13 +3662,13 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3601,13 +3676,13 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3615,13 +3690,13 @@
         <v>21</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3629,13 +3704,13 @@
         <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3643,13 +3718,13 @@
         <v>23</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3657,13 +3732,13 @@
         <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -3671,13 +3746,13 @@
         <v>25</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3685,13 +3760,13 @@
         <v>11</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3699,13 +3774,13 @@
         <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3713,13 +3788,13 @@
         <v>13</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3727,13 +3802,13 @@
         <v>14</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3741,13 +3816,13 @@
         <v>15</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3755,13 +3830,13 @@
         <v>16</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3769,13 +3844,13 @@
         <v>17</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3783,13 +3858,13 @@
         <v>18</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3797,13 +3872,13 @@
         <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3811,13 +3886,13 @@
         <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3825,13 +3900,13 @@
         <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -3839,13 +3914,13 @@
         <v>63</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3853,13 +3928,13 @@
         <v>64</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3867,13 +3942,13 @@
         <v>65</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3881,13 +3956,13 @@
         <v>66</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -3895,13 +3970,13 @@
         <v>67</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3909,13 +3984,13 @@
         <v>28</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3923,13 +3998,13 @@
         <v>29</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3937,13 +4012,13 @@
         <v>32</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3951,13 +4026,13 @@
         <v>33</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3965,13 +4040,13 @@
         <v>34</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3979,13 +4054,13 @@
         <v>35</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3993,13 +4068,13 @@
         <v>36</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -4007,13 +4082,13 @@
         <v>37</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -4021,13 +4096,13 @@
         <v>38</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -4035,13 +4110,13 @@
         <v>39</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -4049,13 +4124,13 @@
         <v>40</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -4063,13 +4138,13 @@
         <v>41</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -4077,13 +4152,13 @@
         <v>42</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -4091,13 +4166,13 @@
         <v>43</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -4105,13 +4180,13 @@
         <v>44</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -4119,13 +4194,13 @@
         <v>45</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -4133,13 +4208,13 @@
         <v>46</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -4147,13 +4222,13 @@
         <v>47</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -4161,13 +4236,13 @@
         <v>48</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -4175,13 +4250,13 @@
         <v>49</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -4189,13 +4264,13 @@
         <v>50</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -4203,13 +4278,13 @@
         <v>51</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -4217,13 +4292,13 @@
         <v>52</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -4231,13 +4306,13 @@
         <v>53</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -4245,13 +4320,13 @@
         <v>54</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -4259,13 +4334,13 @@
         <v>55</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -4273,13 +4348,13 @@
         <v>56</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -4287,13 +4362,13 @@
         <v>57</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -4301,13 +4376,13 @@
         <v>58</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -4315,13 +4390,13 @@
         <v>59</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -4329,13 +4404,13 @@
         <v>60</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -4343,13 +4418,13 @@
         <v>61</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -4357,13 +4432,13 @@
         <v>62</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -4371,13 +4446,13 @@
         <v>68</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -4385,13 +4460,13 @@
         <v>69</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -4399,13 +4474,13 @@
         <v>70</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -4413,13 +4488,13 @@
         <v>71</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -4427,13 +4502,13 @@
         <v>72</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -4441,13 +4516,13 @@
         <v>73</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -4455,16 +4530,16 @@
         <v>74</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -4472,16 +4547,16 @@
         <v>75</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -4489,16 +4564,16 @@
         <v>76</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -4506,16 +4581,16 @@
         <v>77</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -4523,13 +4598,13 @@
         <v>78</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -4540,10 +4615,10 @@
         <v>97</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -4551,13 +4626,13 @@
         <v>80</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -4565,13 +4640,13 @@
         <v>81</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -4579,13 +4654,13 @@
         <v>82</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -4593,13 +4668,13 @@
         <v>83</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -4607,13 +4682,13 @@
         <v>84</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -4621,13 +4696,13 @@
         <v>85</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -4635,13 +4710,13 @@
         <v>86</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -4649,13 +4724,13 @@
         <v>87</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -4663,13 +4738,13 @@
         <v>88</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -4677,13 +4752,13 @@
         <v>89</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -4691,13 +4766,13 @@
         <v>90</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -4705,13 +4780,13 @@
         <v>91</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -4719,377 +4794,377 @@
         <v>92</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -5116,862 +5191,862 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated testing of packets and fixed banning and unbanning of players. Regular cleaning for reading clarity.
</commit_message>
<xml_diff>
--- a/RN and Misc/Packets.xlsx
+++ b/RN and Misc/Packets.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="522">
   <si>
     <t>Message ID</t>
   </si>
@@ -139,18 +139,12 @@
     <t>Buy Items</t>
   </si>
   <si>
-    <t>No menu pops</t>
-  </si>
-  <si>
     <t>Ss</t>
   </si>
   <si>
     <t>Sell Items</t>
   </si>
   <si>
-    <t>up, message is sent</t>
-  </si>
-  <si>
     <t>Sf</t>
   </si>
   <si>
@@ -226,6 +220,9 @@
     <t>Server Announcement</t>
   </si>
   <si>
+    <t>Global Message</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
@@ -274,6 +271,9 @@
     <t>Kick Player</t>
   </si>
   <si>
+    <t>Doesn't revert client to login</t>
+  </si>
+  <si>
     <t>Mwn</t>
   </si>
   <si>
@@ -286,18 +286,27 @@
     <t>Rain</t>
   </si>
   <si>
+    <t>Weather only</t>
+  </si>
+  <si>
     <t>Mws</t>
   </si>
   <si>
     <t>Snow or Hail</t>
   </si>
   <si>
+    <t>changed after</t>
+  </si>
+  <si>
     <t>Mwf</t>
   </si>
   <si>
     <t>Fog</t>
   </si>
   <si>
+    <t>doing a relog</t>
+  </si>
+  <si>
     <t>MwS</t>
   </si>
   <si>
@@ -322,6 +331,9 @@
     <t>Announce Message to Server</t>
   </si>
   <si>
+    <t>Announces to Map</t>
+  </si>
+  <si>
     <t>bm</t>
   </si>
   <si>
@@ -404,6 +416,9 @@
   </si>
   <si>
     <t>World Chat</t>
+  </si>
+  <si>
+    <t>Implement (White + Global)</t>
   </si>
   <si>
     <t>Cl</t>
@@ -1681,8 +1696,8 @@
   </sheetPr>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A13" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F21" activeCellId="0" pane="topLeft" sqref="F21"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A17" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D18" activeCellId="0" pane="topLeft" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1690,7 +1705,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.1122448979592"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.5"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.4132653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.484693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2091836734694"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.4285714285714"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.75510204081633"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.9132653061224"/>
@@ -1982,14 +1997,12 @@
       <c r="C16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G16" s="2"/>
     </row>
@@ -1998,19 +2011,17 @@
         <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="18">
@@ -2018,17 +2029,17 @@
         <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19">
@@ -2036,13 +2047,13 @@
         <v>49</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>8</v>
@@ -2056,10 +2067,10 @@
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
@@ -2074,10 +2085,10 @@
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
@@ -2092,10 +2103,10 @@
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
@@ -2110,10 +2121,10 @@
         <v>18</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
@@ -2128,10 +2139,10 @@
         <v>19</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
@@ -2146,10 +2157,10 @@
         <v>20</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2" t="s">
@@ -2164,10 +2175,10 @@
         <v>21</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2" t="s">
@@ -2182,10 +2193,10 @@
         <v>22</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
@@ -2200,14 +2211,12 @@
         <v>23</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>48</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="D28" s="2"/>
       <c r="E28" s="2" t="s">
         <v>8</v>
       </c>
@@ -2220,12 +2229,14 @@
         <v>24</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
         <v>8</v>
       </c>
@@ -2235,22 +2246,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="30">
       <c r="A30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="E30" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="31">
@@ -2258,17 +2269,17 @@
         <v>26</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="32">
@@ -2276,19 +2287,17 @@
         <v>27</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>72</v>
-      </c>
+      <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="33">
@@ -2296,17 +2305,17 @@
         <v>28</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="34">
@@ -2314,17 +2323,17 @@
         <v>29</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="35">
@@ -2332,17 +2341,17 @@
         <v>30</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="36">
@@ -2350,12 +2359,14 @@
         <v>31</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D36" s="2"/>
       <c r="E36" s="2" t="s">
         <v>8</v>
       </c>
@@ -2378,7 +2389,7 @@
         <v>8</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="38">
@@ -2391,12 +2402,14 @@
       <c r="C38" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D38" s="2"/>
+      <c r="D38" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="E38" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="39">
@@ -2404,17 +2417,19 @@
         <v>32</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D39" s="2"/>
+        <v>91</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="E39" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="40">
@@ -2422,17 +2437,19 @@
         <v>32</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D40" s="2"/>
+        <v>94</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="E40" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="41">
@@ -2440,17 +2457,17 @@
         <v>32</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="42">
@@ -2458,17 +2475,17 @@
         <v>32</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="43">
@@ -2476,17 +2493,17 @@
         <v>33</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="44">
@@ -2494,12 +2511,14 @@
         <v>34</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D44" s="2"/>
+        <v>103</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="E44" s="2" t="s">
         <v>8</v>
       </c>
@@ -2512,10 +2531,10 @@
         <v>35</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2" t="s">
@@ -2530,10 +2549,10 @@
         <v>36</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2" t="s">
@@ -2548,10 +2567,10 @@
         <v>37</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2" t="s">
@@ -2566,10 +2585,10 @@
         <v>38</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2" t="s">
@@ -2584,10 +2603,10 @@
         <v>39</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2" t="s">
@@ -2599,16 +2618,16 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="50">
       <c r="A50" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>8</v>
@@ -2622,10 +2641,10 @@
         <v>40</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2" t="s">
@@ -2640,10 +2659,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2" t="s">
@@ -2658,10 +2677,10 @@
         <v>41</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2" t="s">
@@ -2676,10 +2695,10 @@
         <v>42</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2" t="s">
@@ -2694,10 +2713,10 @@
         <v>43</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2" t="s">
@@ -2712,10 +2731,10 @@
         <v>44</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
@@ -2730,10 +2749,10 @@
         <v>45</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2" t="s">
@@ -2748,13 +2767,13 @@
         <v>46</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>48</v>
+        <v>133</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>8</v>
@@ -2768,10 +2787,10 @@
         <v>46</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2" t="s">
@@ -2786,10 +2805,10 @@
         <v>46</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2" t="s">
@@ -2804,10 +2823,10 @@
         <v>47</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2" t="s">
@@ -2822,10 +2841,10 @@
         <v>48</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2" t="s">
@@ -2837,16 +2856,16 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="63">
       <c r="A63" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>8</v>
@@ -2873,8 +2892,8 @@
   </sheetPr>
   <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A57" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F82" activeCellId="0" pane="topLeft" sqref="F82"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C1" activeCellId="0" pane="topLeft" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2920,10 +2939,10 @@
         <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>15</v>
@@ -2934,13 +2953,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>15</v>
@@ -2951,13 +2970,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>15</v>
@@ -2968,13 +2987,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>15</v>
@@ -2985,13 +3004,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>15</v>
@@ -3002,13 +3021,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>15</v>
@@ -3019,13 +3038,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>15</v>
@@ -3036,13 +3055,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>15</v>
@@ -3059,7 +3078,7 @@
         <v>35</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>15</v>
@@ -3070,13 +3089,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>15</v>
@@ -3087,13 +3106,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>15</v>
@@ -3104,13 +3123,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>15</v>
@@ -3121,13 +3140,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>15</v>
@@ -3138,13 +3157,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>15</v>
@@ -3158,10 +3177,10 @@
         <v>38</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>15</v>
@@ -3172,13 +3191,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>15</v>
@@ -3189,13 +3208,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>15</v>
@@ -3206,13 +3225,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>15</v>
@@ -3223,13 +3242,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>15</v>
@@ -3240,13 +3259,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>15</v>
@@ -3257,13 +3276,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>15</v>
@@ -3274,13 +3293,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>15</v>
@@ -3291,13 +3310,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>15</v>
@@ -3308,13 +3327,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>15</v>
@@ -3325,13 +3344,13 @@
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>15</v>
@@ -3342,13 +3361,13 @@
         <v>24</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>15</v>
@@ -3359,13 +3378,13 @@
         <v>24</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>15</v>
@@ -3376,13 +3395,13 @@
         <v>25</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>15</v>
@@ -3393,13 +3412,13 @@
         <v>26</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>15</v>
@@ -3410,13 +3429,13 @@
         <v>27</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>15</v>
@@ -3427,13 +3446,13 @@
         <v>28</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>15</v>
@@ -3444,13 +3463,13 @@
         <v>29</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>15</v>
@@ -3461,13 +3480,13 @@
         <v>30</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>15</v>
@@ -3478,13 +3497,13 @@
         <v>31</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>15</v>
@@ -3495,13 +3514,13 @@
         <v>32</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>15</v>
@@ -3512,13 +3531,13 @@
         <v>33</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>15</v>
@@ -3529,13 +3548,13 @@
         <v>33</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>15</v>
@@ -3546,13 +3565,13 @@
         <v>34</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>15</v>
@@ -3563,13 +3582,13 @@
         <v>34</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>15</v>
@@ -3580,13 +3599,13 @@
         <v>35</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>15</v>
@@ -3597,13 +3616,13 @@
         <v>36</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>15</v>
@@ -3614,13 +3633,13 @@
         <v>37</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>15</v>
@@ -3631,13 +3650,13 @@
         <v>38</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>15</v>
@@ -3648,13 +3667,13 @@
         <v>39</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>15</v>
@@ -3668,10 +3687,10 @@
         <v>26</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>15</v>
@@ -3685,10 +3704,10 @@
         <v>28</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>15</v>
@@ -3699,13 +3718,13 @@
         <v>42</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>15</v>
@@ -3716,13 +3735,13 @@
         <v>43</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>15</v>
@@ -3733,13 +3752,13 @@
         <v>44</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>15</v>
@@ -3750,13 +3769,13 @@
         <v>45</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>15</v>
@@ -3767,13 +3786,13 @@
         <v>89</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>15</v>
@@ -3784,13 +3803,13 @@
         <v>46</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>15</v>
@@ -3801,13 +3820,13 @@
         <v>47</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>15</v>
@@ -3818,13 +3837,13 @@
         <v>48</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>15</v>
@@ -3835,13 +3854,13 @@
         <v>49</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>15</v>
@@ -3852,13 +3871,13 @@
         <v>50</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>9</v>
@@ -3869,13 +3888,13 @@
         <v>51</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>15</v>
@@ -3886,13 +3905,13 @@
         <v>52</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>15</v>
@@ -3903,13 +3922,13 @@
         <v>52</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>15</v>
@@ -3920,13 +3939,13 @@
         <v>53</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>15</v>
@@ -3937,13 +3956,13 @@
         <v>54</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>15</v>
@@ -3954,13 +3973,13 @@
         <v>55</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>15</v>
@@ -3971,13 +3990,13 @@
         <v>56</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>15</v>
@@ -3988,13 +4007,13 @@
         <v>57</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>15</v>
@@ -4005,13 +4024,13 @@
         <v>57</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>88</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>15</v>
@@ -4022,13 +4041,13 @@
         <v>57</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>15</v>
@@ -4039,13 +4058,13 @@
         <v>57</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>15</v>
@@ -4056,13 +4075,13 @@
         <v>57</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>15</v>
@@ -4073,13 +4092,13 @@
         <v>88</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>15</v>
@@ -4090,13 +4109,13 @@
         <v>58</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>15</v>
@@ -4107,16 +4126,16 @@
         <v>59</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>15</v>
@@ -4127,16 +4146,16 @@
         <v>60</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>15</v>
@@ -4147,16 +4166,16 @@
         <v>61</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>15</v>
@@ -4167,16 +4186,16 @@
         <v>62</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>15</v>
@@ -4187,13 +4206,13 @@
         <v>63</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>15</v>
@@ -4207,10 +4226,10 @@
         <v>18</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>15</v>
@@ -4221,13 +4240,13 @@
         <v>65</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>15</v>
@@ -4238,13 +4257,13 @@
         <v>66</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>15</v>
@@ -4255,13 +4274,13 @@
         <v>67</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>15</v>
@@ -4272,13 +4291,13 @@
         <v>68</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>15</v>
@@ -4289,13 +4308,13 @@
         <v>69</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>15</v>
@@ -4306,13 +4325,13 @@
         <v>70</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>15</v>
@@ -4320,16 +4339,16 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="84">
       <c r="A84" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>15</v>
@@ -4337,16 +4356,16 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="85">
       <c r="A85" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>15</v>
@@ -4357,13 +4376,13 @@
         <v>71</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>15</v>
@@ -4374,13 +4393,13 @@
         <v>72</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>15</v>
@@ -4391,13 +4410,13 @@
         <v>73</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>15</v>
@@ -4408,13 +4427,13 @@
         <v>73</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>15</v>
@@ -4425,13 +4444,13 @@
         <v>74</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>15</v>
@@ -4442,13 +4461,13 @@
         <v>75</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>15</v>
@@ -4459,13 +4478,13 @@
         <v>76</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>15</v>
@@ -4476,13 +4495,13 @@
         <v>77</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>15</v>
@@ -4493,13 +4512,13 @@
         <v>78</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>15</v>
@@ -4508,13 +4527,13 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="95">
       <c r="A95" s="5"/>
       <c r="B95" s="2" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>15</v>
@@ -4525,13 +4544,13 @@
         <v>79</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>15</v>
@@ -4542,13 +4561,13 @@
         <v>80</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>15</v>
@@ -4559,13 +4578,13 @@
         <v>81</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F98" s="2" t="s">
         <v>15</v>
@@ -4576,13 +4595,13 @@
         <v>82</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>15</v>
@@ -4593,13 +4612,13 @@
         <v>90</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F100" s="2" t="s">
         <v>15</v>
@@ -4610,13 +4629,13 @@
         <v>91</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F101" s="2" t="s">
         <v>15</v>
@@ -4625,13 +4644,13 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="102">
       <c r="A102" s="5"/>
       <c r="B102" s="2" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>15</v>
@@ -4640,13 +4659,13 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="103">
       <c r="A103" s="5"/>
       <c r="B103" s="2" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>15</v>
@@ -4655,13 +4674,13 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="104">
       <c r="A104" s="5"/>
       <c r="B104" s="2" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F104" s="2" t="s">
         <v>15</v>
@@ -4670,13 +4689,13 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="105">
       <c r="A105" s="5"/>
       <c r="B105" s="2" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F105" s="2" t="s">
         <v>15</v>
@@ -4685,13 +4704,13 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="106">
       <c r="A106" s="5"/>
       <c r="B106" s="2" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>15</v>
@@ -4702,13 +4721,13 @@
         <v>83</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F107" s="2" t="s">
         <v>15</v>
@@ -4719,13 +4738,13 @@
         <v>84</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F108" s="2" t="s">
         <v>15</v>
@@ -4736,13 +4755,13 @@
         <v>85</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F109" s="2" t="s">
         <v>15</v>
@@ -4753,13 +4772,13 @@
         <v>86</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F110" s="2" t="s">
         <v>15</v>
@@ -4770,13 +4789,13 @@
         <v>87</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F111" s="2" t="s">
         <v>15</v>
@@ -4787,13 +4806,13 @@
         <v>87</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F112" s="2" t="s">
         <v>15</v>
@@ -4804,13 +4823,13 @@
         <v>87</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F113" s="2" t="s">
         <v>15</v>
@@ -4821,13 +4840,13 @@
         <v>87</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F114" s="2" t="s">
         <v>15</v>
@@ -4838,13 +4857,13 @@
         <v>87</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F115" s="2" t="s">
         <v>15</v>
@@ -4855,13 +4874,13 @@
         <v>87</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F116" s="2" t="s">
         <v>15</v>
@@ -4897,862 +4916,862 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1">
       <c r="A1" s="6" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="6" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="A3" s="6" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="4">
       <c r="A4" s="6" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="5">
       <c r="A5" s="6" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="6">
       <c r="A6" s="6" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="6" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="8">
       <c r="A8" s="6" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="9">
       <c r="A9" s="6" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="10">
       <c r="A10" s="6" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="11">
       <c r="A11" s="6" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="12">
       <c r="A12" s="6" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="13">
       <c r="A13" s="6" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="14">
       <c r="A14" s="6" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="15">
       <c r="A15" s="6" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="16">
       <c r="A16" s="6" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="17">
       <c r="A17" s="6" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="18">
       <c r="A18" s="6" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19">
       <c r="A19" s="6" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="20">
       <c r="A20" s="6" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="21">
       <c r="A21" s="6" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="22">
       <c r="A22" s="6" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="23">
       <c r="A23" s="6" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="24">
       <c r="A24" s="6" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="25">
       <c r="A25" s="6" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="26">
       <c r="A26" s="6" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="27">
       <c r="A27" s="6" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="28">
       <c r="A28" s="6" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="29">
       <c r="A29" s="6" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="30">
       <c r="A30" s="6" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="31">
       <c r="A31" s="6" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="32">
       <c r="A32" s="6" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="33">
       <c r="A33" s="6" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="34">
       <c r="A34" s="6" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="35">
       <c r="A35" s="6" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="36">
       <c r="A36" s="6" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="37">
       <c r="A37" s="6" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="38">
       <c r="A38" s="6" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="39">
       <c r="A39" s="6" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="40">
       <c r="A40" s="6" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="41">
       <c r="A41" s="6" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="42">
       <c r="A42" s="6" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="43">
       <c r="A43" s="6" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="44">
       <c r="A44" s="6" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="45">
       <c r="A45" s="6" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="46">
       <c r="A46" s="6" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="47">
       <c r="A47" s="6" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="48">
       <c r="A48" s="6" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="49">
       <c r="A49" s="6" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="50">
       <c r="A50" s="6" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="51">
       <c r="A51" s="6" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="52">
       <c r="A52" s="6" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="53">
       <c r="A53" s="6" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="54">
       <c r="A54" s="6" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="55">
       <c r="A55" s="6" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="56">
       <c r="A56" s="6" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="57">
       <c r="A57" s="6" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="58">
       <c r="A58" s="6" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="60">
       <c r="A60" s="6" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="61">
       <c r="A61" s="6" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="62">
       <c r="A62" s="6" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="63">
       <c r="A63" s="6" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="64">
       <c r="A64" s="6" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="65">
       <c r="A65" s="6" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="66">
       <c r="A66" s="6" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="67">
       <c r="A67" s="6" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="68">
       <c r="A68" s="6" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="69">
       <c r="A69" s="6" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="70">
       <c r="A70" s="6" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="71">
       <c r="A71" s="6" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="72">
       <c r="A72" s="6" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="73">
       <c r="A73" s="6" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="74">
       <c r="A74" s="6" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="75">
       <c r="A75" s="6" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="76">
       <c r="A76" s="6" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="77">
       <c r="A77" s="6" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="78">
       <c r="A78" s="6" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="79">
       <c r="A79" s="6" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="80">
       <c r="A80" s="6" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="81">
       <c r="A81" s="6" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="82">
       <c r="A82" s="6" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="83">
       <c r="A83" s="6" t="s">
-        <v>428</v>
+        <v>433</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="84">
       <c r="A84" s="6" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="85">
       <c r="A85" s="6" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="86">
       <c r="A86" s="6" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="87">
       <c r="A87" s="6" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="88">
       <c r="A88" s="6" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="89">
       <c r="A89" s="6" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="90">
       <c r="A90" s="6" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="91">
       <c r="A91" s="6" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="92">
       <c r="A92" s="6" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="93">
       <c r="A93" s="6" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="94">
       <c r="A94" s="6" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="95">
       <c r="A95" s="6" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="96">
       <c r="A96" s="6" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="97">
       <c r="A97" s="6" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="98">
       <c r="A98" s="6" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="99">
       <c r="A99" s="6" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="100">
       <c r="A100" s="6" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="101">
       <c r="A101" s="6" t="s">
-        <v>446</v>
+        <v>451</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="102">
       <c r="A102" s="6" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="103">
       <c r="A103" s="6" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="104">
       <c r="A104" s="6" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="105">
       <c r="A105" s="6" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="106">
       <c r="A106" s="6" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="107">
       <c r="A107" s="6" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="108">
       <c r="A108" s="6" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="109">
       <c r="A109" s="6" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="110">
       <c r="A110" s="6" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="111">
       <c r="A111" s="6" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="112">
       <c r="A112" s="6" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="113">
       <c r="A113" s="6" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="114">
       <c r="A114" s="6" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="115">
       <c r="A115" s="6" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="116">
       <c r="A116" s="6" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="117">
       <c r="A117" s="6" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="118">
       <c r="A118" s="6" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="119">
       <c r="A119" s="6" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="120">
       <c r="A120" s="6" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="121">
       <c r="A121" s="6" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="122">
       <c r="A122" s="6" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="123">
       <c r="A123" s="6" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="124">
       <c r="A124" s="6" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="125">
       <c r="A125" s="6" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="126">
       <c r="A126" s="6" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="127">
       <c r="A127" s="6" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="128">
       <c r="A128" s="6" t="s">
-        <v>473</v>
+        <v>478</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="129">
       <c r="A129" s="6" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="130">
       <c r="A130" s="6" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="131">
       <c r="A131" s="6" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="132">
       <c r="A132" s="6" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="133">
       <c r="A133" s="6" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="134">
       <c r="A134" s="6" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="135">
       <c r="A135" s="6" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="136">
       <c r="A136" s="6" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="137">
       <c r="A137" s="6" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="138">
       <c r="A138" s="6" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="139">
       <c r="A139" s="6" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="140">
       <c r="A140" s="6" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="141">
       <c r="A141" s="6" t="s">
-        <v>486</v>
+        <v>491</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="142">
       <c r="A142" s="6" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="143">
       <c r="A143" s="6" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="144">
       <c r="A144" s="6" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="145">
       <c r="A145" s="6" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="146">
       <c r="A146" s="6" t="s">
-        <v>491</v>
+        <v>496</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="147">
       <c r="A147" s="6" t="s">
-        <v>492</v>
+        <v>497</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="148">
       <c r="A148" s="6" t="s">
-        <v>493</v>
+        <v>498</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="149">
       <c r="A149" s="6" t="s">
-        <v>494</v>
+        <v>499</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="150">
       <c r="A150" s="6" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="151">
       <c r="A151" s="6" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="152">
       <c r="A152" s="6" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="153">
       <c r="A153" s="6" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="154">
       <c r="A154" s="6" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="155">
       <c r="A155" s="6" t="s">
-        <v>500</v>
+        <v>505</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="156">
       <c r="A156" s="6" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="157">
       <c r="A157" s="6" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="158">
       <c r="A158" s="6" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="159">
       <c r="A159" s="6" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="160">
       <c r="A160" s="6" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="161">
       <c r="A161" s="6" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="162">
       <c r="A162" s="6" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="163">
       <c r="A163" s="6" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="164">
       <c r="A164" s="6" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="165">
       <c r="A165" s="6" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="166">
       <c r="A166" s="6" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="167">
       <c r="A167" s="6" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="168">
       <c r="A168" s="6" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="169">
       <c r="A169" s="6" t="s">
-        <v>512</v>
+        <v>517</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="170">
       <c r="A170" s="6" t="s">
-        <v>513</v>
+        <v>518</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="171">
       <c r="A171" s="6" t="s">
-        <v>514</v>
+        <v>519</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="172">
       <c r="A172" s="6" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="173">
       <c r="A173" s="6" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced all the seperate level packets with one packet and updated neccessary 'documentation'.
</commit_message>
<xml_diff>
--- a/RN and Misc/Packets.xlsx
+++ b/RN and Misc/Packets.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="526">
   <si>
     <t>Message ID</t>
   </si>
@@ -784,6 +784,9 @@
     <t>Coordinating Level Up</t>
   </si>
   <si>
+    <t>Skill Level Up</t>
+  </si>
+  <si>
     <t>cWn</t>
   </si>
   <si>
@@ -970,9 +973,6 @@
     <t>Remove Item from Bag</t>
   </si>
   <si>
-    <t>82</t>
-  </si>
-  <si>
     <t>r!0</t>
   </si>
   <si>
@@ -1081,13 +1081,7 @@
     <t>Trade Offer Invalid</t>
   </si>
   <si>
-    <t>95</t>
-  </si>
-  <si>
     <t>Boat Travel</t>
-  </si>
-  <si>
-    <t>96</t>
   </si>
   <si>
     <t>Travel Event</t>
@@ -1690,12 +1684,12 @@
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
   </cellXfs>
@@ -1718,7 +1712,7 @@
   <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D19" activeCellId="0" pane="topLeft" sqref="D19"/>
+      <selection activeCell="C26" activeCellId="0" pane="topLeft" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2909,10 +2903,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G120"/>
+  <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A81" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C117" activeCellId="0" pane="topLeft" sqref="C117"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A45" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F65" activeCellId="0" pane="topLeft" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2920,15 +2914,15 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="11.1122448979592"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="4" width="6.5"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="4" width="31.7397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.75510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="8.75510204081633"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="4" width="14.4285714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.75510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.1122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.75510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="8.75510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="11.1122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="5" width="8.75510204081633"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -2951,7 +2945,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
-      <c r="A2" s="5" t="n">
+      <c r="A2" s="6" t="n">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2968,7 +2962,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="3">
-      <c r="A3" s="5" t="n">
+      <c r="A3" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -2985,7 +2979,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="4">
-      <c r="A4" s="5" t="n">
+      <c r="A4" s="6" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -3002,7 +2996,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="5">
-      <c r="A5" s="5" t="n">
+      <c r="A5" s="6" t="n">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -3019,7 +3013,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="6">
-      <c r="A6" s="5" t="n">
+      <c r="A6" s="6" t="n">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -3036,7 +3030,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="7">
-      <c r="A7" s="5" t="n">
+      <c r="A7" s="6" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -3053,7 +3047,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="8">
-      <c r="A8" s="5" t="n">
+      <c r="A8" s="6" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -3070,7 +3064,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="9">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="6" t="n">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -3087,7 +3081,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="10">
-      <c r="A10" s="5" t="n">
+      <c r="A10" s="6" t="n">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -3104,7 +3098,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="11">
-      <c r="A11" s="5" t="n">
+      <c r="A11" s="6" t="n">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -3121,7 +3115,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="12">
-      <c r="A12" s="5" t="n">
+      <c r="A12" s="6" t="n">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -3138,7 +3132,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="13">
-      <c r="A13" s="5" t="n">
+      <c r="A13" s="6" t="n">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -3155,7 +3149,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="14">
-      <c r="A14" s="5" t="n">
+      <c r="A14" s="6" t="n">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -3172,7 +3166,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="15">
-      <c r="A15" s="5" t="n">
+      <c r="A15" s="6" t="n">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -3189,7 +3183,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="16">
-      <c r="A16" s="5" t="n">
+      <c r="A16" s="6" t="n">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -3206,7 +3200,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="17">
-      <c r="A17" s="5" t="n">
+      <c r="A17" s="6" t="n">
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -3223,7 +3217,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="18">
-      <c r="A18" s="5" t="n">
+      <c r="A18" s="6" t="n">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -3240,7 +3234,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19">
-      <c r="A19" s="5" t="n">
+      <c r="A19" s="6" t="n">
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -3257,7 +3251,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="20">
-      <c r="A20" s="5" t="n">
+      <c r="A20" s="6" t="n">
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -3274,7 +3268,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="21">
-      <c r="A21" s="5" t="n">
+      <c r="A21" s="6" t="n">
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -3291,7 +3285,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="22">
-      <c r="A22" s="5" t="n">
+      <c r="A22" s="6" t="n">
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -3308,7 +3302,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="23">
-      <c r="A23" s="5" t="n">
+      <c r="A23" s="6" t="n">
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -3325,7 +3319,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="24">
-      <c r="A24" s="5" t="n">
+      <c r="A24" s="6" t="n">
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -3342,7 +3336,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="25">
-      <c r="A25" s="5" t="n">
+      <c r="A25" s="6" t="n">
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -3359,7 +3353,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="26">
-      <c r="A26" s="5" t="n">
+      <c r="A26" s="6" t="n">
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -3376,7 +3370,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="27">
-      <c r="A27" s="5" t="n">
+      <c r="A27" s="6" t="n">
         <v>24</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -3393,7 +3387,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="28">
-      <c r="A28" s="5" t="n">
+      <c r="A28" s="6" t="n">
         <v>24</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -3410,7 +3404,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="29">
-      <c r="A29" s="5" t="n">
+      <c r="A29" s="6" t="n">
         <v>25</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -3427,7 +3421,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="30">
-      <c r="A30" s="5" t="n">
+      <c r="A30" s="6" t="n">
         <v>26</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -3444,7 +3438,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="31">
-      <c r="A31" s="5" t="n">
+      <c r="A31" s="6" t="n">
         <v>27</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -3461,7 +3455,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="32">
-      <c r="A32" s="5" t="n">
+      <c r="A32" s="6" t="n">
         <v>28</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -3478,7 +3472,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="33">
-      <c r="A33" s="5" t="n">
+      <c r="A33" s="6" t="n">
         <v>29</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -3495,7 +3489,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="34">
-      <c r="A34" s="5" t="n">
+      <c r="A34" s="6" t="n">
         <v>30</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -3512,7 +3506,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="35">
-      <c r="A35" s="5" t="n">
+      <c r="A35" s="6" t="n">
         <v>31</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -3529,7 +3523,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="36">
-      <c r="A36" s="5" t="n">
+      <c r="A36" s="6" t="n">
         <v>32</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -3546,7 +3540,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="37">
-      <c r="A37" s="5" t="n">
+      <c r="A37" s="6" t="n">
         <v>33</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -3563,7 +3557,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="38">
-      <c r="A38" s="5" t="n">
+      <c r="A38" s="6" t="n">
         <v>33</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -3580,7 +3574,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="39">
-      <c r="A39" s="5" t="n">
+      <c r="A39" s="6" t="n">
         <v>34</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -3597,7 +3591,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="40">
-      <c r="A40" s="5" t="n">
+      <c r="A40" s="6" t="n">
         <v>34</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -3614,7 +3608,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="41">
-      <c r="A41" s="5" t="n">
+      <c r="A41" s="6" t="n">
         <v>35</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -3631,7 +3625,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="42">
-      <c r="A42" s="5" t="n">
+      <c r="A42" s="6" t="n">
         <v>36</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -3648,7 +3642,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="43">
-      <c r="A43" s="5" t="n">
+      <c r="A43" s="6" t="n">
         <v>37</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -3665,7 +3659,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="44">
-      <c r="A44" s="5" t="n">
+      <c r="A44" s="6" t="n">
         <v>38</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -3682,7 +3676,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="45">
-      <c r="A45" s="5" t="n">
+      <c r="A45" s="6" t="n">
         <v>39</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -3699,7 +3693,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="46">
-      <c r="A46" s="5" t="n">
+      <c r="A46" s="6" t="n">
         <v>40</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -3716,7 +3710,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="47">
-      <c r="A47" s="5" t="n">
+      <c r="A47" s="6" t="n">
         <v>41</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -3733,7 +3727,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="48">
-      <c r="A48" s="5" t="n">
+      <c r="A48" s="6" t="n">
         <v>42</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -3750,7 +3744,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="49">
-      <c r="A49" s="5" t="n">
+      <c r="A49" s="6" t="n">
         <v>43</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -3767,7 +3761,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="50">
-      <c r="A50" s="5" t="n">
+      <c r="A50" s="6" t="n">
         <v>44</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -3784,7 +3778,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="51">
-      <c r="A51" s="5" t="n">
+      <c r="A51" s="6" t="n">
         <v>45</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -3801,7 +3795,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="52">
-      <c r="A52" s="5" t="n">
+      <c r="A52" s="6" t="n">
         <v>46</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -3818,7 +3812,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="53">
-      <c r="A53" s="5" t="n">
+      <c r="A53" s="6" t="n">
         <v>47</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -3835,7 +3829,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="54">
-      <c r="A54" s="5" t="n">
+      <c r="A54" s="6" t="n">
         <v>48</v>
       </c>
       <c r="B54" s="2" t="s">
@@ -3852,7 +3846,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="55">
-      <c r="A55" s="5" t="n">
+      <c r="A55" s="6" t="n">
         <v>49</v>
       </c>
       <c r="B55" s="2" t="s">
@@ -3869,7 +3863,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="56">
-      <c r="A56" s="5" t="n">
+      <c r="A56" s="6" t="n">
         <v>50</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -3886,7 +3880,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="57">
-      <c r="A57" s="5" t="n">
+      <c r="A57" s="6" t="n">
         <v>51</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -3903,7 +3897,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="58">
-      <c r="A58" s="5" t="n">
+      <c r="A58" s="6" t="n">
         <v>52</v>
       </c>
       <c r="B58" s="2" t="s">
@@ -3920,7 +3914,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="59">
-      <c r="A59" s="5" t="n">
+      <c r="A59" s="6" t="n">
         <v>52</v>
       </c>
       <c r="B59" s="2" t="s">
@@ -3937,8 +3931,8 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="60">
-      <c r="A60" s="5" t="n">
-        <v>53</v>
+      <c r="A60" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>247</v>
@@ -3954,8 +3948,8 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="61">
-      <c r="A61" s="5" t="n">
-        <v>54</v>
+      <c r="A61" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>249</v>
@@ -3971,8 +3965,8 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="62">
-      <c r="A62" s="5" t="n">
-        <v>55</v>
+      <c r="A62" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>251</v>
@@ -3988,8 +3982,8 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="63">
-      <c r="A63" s="5" t="n">
-        <v>56</v>
+      <c r="A63" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>253</v>
@@ -4006,31 +4000,31 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="64">
       <c r="A64" s="5" t="n">
+        <v>53</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="65">
+      <c r="A65" s="6" t="n">
         <v>57</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="C64" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="E64" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="65">
-      <c r="A65" s="5" t="n">
-        <v>57</v>
-      </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="E65" s="2" t="s">
         <v>145</v>
       </c>
@@ -4039,32 +4033,32 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="66">
-      <c r="A66" s="5" t="n">
+      <c r="A66" s="6" t="n">
         <v>57</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>258</v>
       </c>
       <c r="C66" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="67">
+      <c r="A67" s="6" t="n">
+        <v>57</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="E66" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="67">
-      <c r="A67" s="5" t="n">
-        <v>57</v>
-      </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="C67" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="E67" s="2" t="s">
         <v>145</v>
       </c>
@@ -4073,14 +4067,14 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="68">
-      <c r="A68" s="5" t="n">
+      <c r="A68" s="6" t="n">
         <v>57</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>261</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>145</v>
@@ -4090,51 +4084,48 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="69">
-      <c r="A69" s="5" t="n">
-        <v>58</v>
+      <c r="A69" s="6" t="n">
+        <v>57</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>262</v>
       </c>
       <c r="C69" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="70">
+      <c r="A70" s="6" t="n">
+        <v>58</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="E69" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="70">
-      <c r="A70" s="5" t="n">
+      <c r="C70" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="71">
+      <c r="A71" s="6" t="n">
         <v>59</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="C70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="71">
-      <c r="A71" s="5" t="n">
-        <v>60</v>
-      </c>
-      <c r="B71" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>267</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>14</v>
@@ -4147,14 +4138,14 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="72">
-      <c r="A72" s="5" t="n">
-        <v>61</v>
+      <c r="A72" s="6" t="n">
+        <v>60</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>269</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>14</v>
@@ -4167,14 +4158,14 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="73">
-      <c r="A73" s="5" t="n">
-        <v>62</v>
+      <c r="A73" s="6" t="n">
+        <v>61</v>
       </c>
       <c r="B73" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>271</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>14</v>
@@ -4187,28 +4178,31 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="74">
-      <c r="A74" s="5" t="n">
+      <c r="A74" s="6" t="n">
+        <v>62</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="75">
+      <c r="A75" s="6" t="n">
         <v>63</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="C74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="75">
-      <c r="A75" s="5" t="n">
-        <v>64</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>274</v>
@@ -4221,677 +4215,677 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="76">
-      <c r="A76" s="5" t="n">
+      <c r="A76" s="6" t="n">
+        <v>64</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="77">
+      <c r="A77" s="6" t="n">
         <v>65</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="C76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="E76" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="77">
-      <c r="A77" s="5" t="n">
+      <c r="C77" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="78">
+      <c r="A78" s="6" t="n">
         <v>66</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="C77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="E77" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="78">
-      <c r="A78" s="5" t="n">
+      <c r="C78" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="79">
+      <c r="A79" s="6" t="n">
         <v>67</v>
       </c>
-      <c r="B78" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="C78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="E78" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="79">
-      <c r="A79" s="5" t="n">
+      <c r="C79" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="80">
+      <c r="A80" s="6" t="n">
         <v>68</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="C79" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="E79" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="80">
-      <c r="A80" s="5" t="n">
+      <c r="C80" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="81">
+      <c r="A81" s="6" t="n">
         <v>69</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="C80" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="E80" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="81">
-      <c r="A81" s="5" t="n">
+      <c r="C81" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="82">
+      <c r="A82" s="6" t="n">
         <v>70</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="C81" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="E81" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="82">
-      <c r="A82" s="5" t="s">
+      <c r="C82" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="83">
+      <c r="A83" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="C82" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="E82" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="83">
-      <c r="A83" s="5" t="s">
+      <c r="C83" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="84">
+      <c r="A84" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="C83" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="E83" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="84">
-      <c r="A84" s="5" t="n">
+      <c r="C84" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="85">
+      <c r="A85" s="6" t="n">
         <v>71</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="C84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="E84" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="85">
-      <c r="A85" s="5" t="n">
+      <c r="C85" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="86">
+      <c r="A86" s="6" t="n">
         <v>72</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="C85" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="E85" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="86">
-      <c r="A86" s="5" t="n">
+      <c r="C86" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="87">
+      <c r="A87" s="6" t="n">
         <v>73</v>
       </c>
-      <c r="B86" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="C86" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="E86" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="87">
-      <c r="A87" s="5" t="n">
+      <c r="C87" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="88">
+      <c r="A88" s="6" t="n">
         <v>73</v>
       </c>
-      <c r="B87" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="C87" s="2" t="s">
+      <c r="B88" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="E87" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="88">
-      <c r="A88" s="5" t="n">
+      <c r="C88" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="89">
+      <c r="A89" s="6" t="n">
         <v>74</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="C88" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="E88" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="89">
-      <c r="A89" s="5" t="n">
+      <c r="C89" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="90">
+      <c r="A90" s="6" t="n">
         <v>75</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="C89" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="E89" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="90">
-      <c r="A90" s="5" t="n">
+      <c r="C90" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="91">
+      <c r="A91" s="6" t="n">
         <v>76</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="C90" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="E90" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="91">
-      <c r="A91" s="5" t="n">
+      <c r="C91" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="92">
+      <c r="A92" s="6" t="n">
         <v>77</v>
       </c>
-      <c r="B91" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="C91" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="E91" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="92">
-      <c r="A92" s="5" t="n">
+      <c r="C92" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="93">
+      <c r="A93" s="6" t="n">
         <v>78</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B93" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="94">
+      <c r="A94" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="95">
+      <c r="A95" s="6" t="n">
+        <v>79</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="96">
+      <c r="A96" s="6" t="n">
+        <v>80</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="97">
+      <c r="A97" s="6" t="n">
+        <v>81</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="98">
+      <c r="A98" s="6" t="n">
+        <v>82</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="99">
+      <c r="A99" s="6" t="n">
+        <v>82</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="100">
+      <c r="A100" s="6" t="n">
+        <v>82</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="101">
+      <c r="A101" s="6" t="n">
+        <v>82</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="102">
+      <c r="A102" s="6" t="n">
+        <v>82</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="103">
+      <c r="A103" s="6" t="n">
+        <v>83</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="104">
+      <c r="A104" s="6" t="n">
+        <v>84</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="105">
+      <c r="A105" s="6" t="n">
+        <v>85</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="106">
+      <c r="A106" s="6" t="n">
+        <v>86</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="107">
+      <c r="A107" s="6" t="n">
+        <v>87</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C107" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="C92" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="93">
-      <c r="A93" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="94">
-      <c r="A94" s="5" t="n">
-        <v>79</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="95">
-      <c r="A95" s="5" t="n">
-        <v>80</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="96">
-      <c r="A96" s="5" t="n">
-        <v>81</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="97">
-      <c r="A97" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="98">
-      <c r="A98" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="99">
-      <c r="A99" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="100">
-      <c r="A100" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="101">
-      <c r="A101" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="102">
-      <c r="A102" s="5" t="n">
-        <v>83</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E102" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="103">
-      <c r="A103" s="5" t="n">
-        <v>84</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E103" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F103" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="104">
-      <c r="A104" s="5" t="n">
-        <v>85</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E104" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="105">
-      <c r="A105" s="5" t="n">
-        <v>86</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="106">
-      <c r="A106" s="5" t="n">
+      <c r="E107" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="108">
+      <c r="A108" s="6" t="n">
         <v>87</v>
       </c>
-      <c r="B106" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="E106" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="107">
-      <c r="A107" s="5" t="n">
+      <c r="B108" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="109">
+      <c r="A109" s="6" t="n">
         <v>87</v>
       </c>
-      <c r="B107" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="E107" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="108">
-      <c r="A108" s="5" t="n">
+      <c r="B109" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="110">
+      <c r="A110" s="6" t="n">
         <v>87</v>
       </c>
-      <c r="B108" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F108" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="109">
-      <c r="A109" s="5" t="n">
+      <c r="B110" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="111">
+      <c r="A111" s="6" t="n">
         <v>87</v>
       </c>
-      <c r="B109" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="E109" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="110">
-      <c r="A110" s="5" t="n">
+      <c r="B111" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="112">
+      <c r="A112" s="6" t="n">
         <v>87</v>
       </c>
-      <c r="B110" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="E110" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F110" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="111">
-      <c r="A111" s="5" t="n">
-        <v>87</v>
-      </c>
-      <c r="B111" s="2" t="s">
+      <c r="B112" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="C112" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="E111" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F111" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="112">
-      <c r="A112" s="5" t="n">
+      <c r="E112" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="113">
+      <c r="A113" s="6" t="n">
         <v>88</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B113" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="C113" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="E112" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F112" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="113">
-      <c r="A113" s="5" t="n">
+      <c r="E113" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="114">
+      <c r="A114" s="6" t="n">
         <v>89</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B114" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="C114" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E113" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F113" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="114">
-      <c r="A114" s="5" t="n">
+      <c r="E114" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="115">
+      <c r="A115" s="6" t="n">
         <v>90</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B115" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="C115" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="E114" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F114" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="115">
-      <c r="A115" s="5" t="n">
-        <v>91</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>349</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>145</v>
@@ -4902,68 +4896,65 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="116">
       <c r="A116" s="6" t="n">
+        <v>91</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="117">
+      <c r="A117" s="5" t="n">
         <v>92</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B117" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="C117" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="E116" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="117">
-      <c r="A117" s="6" t="n">
+      <c r="E117" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="118">
+      <c r="A118" s="5" t="n">
         <v>93</v>
       </c>
-      <c r="B117" s="6" t="s">
+      <c r="B118" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C117" s="6" t="s">
+      <c r="C118" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="D117" s="6"/>
-      <c r="E117" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F117" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="118">
-      <c r="A118" s="6" t="n">
+      <c r="E118" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="119">
+      <c r="A119" s="5" t="n">
         <v>94</v>
       </c>
-      <c r="B118" s="6" t="s">
+      <c r="B119" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C118" s="6" t="s">
+      <c r="C119" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="D118" s="6"/>
-      <c r="E118" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F118" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="119">
-      <c r="A119" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="B119" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C119" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="D119" s="6"/>
       <c r="E119" s="2" t="s">
         <v>145</v>
       </c>
@@ -4972,20 +4963,36 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="120">
-      <c r="A120" s="3" t="s">
-        <v>356</v>
+      <c r="A120" s="3" t="n">
+        <v>95</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="D120" s="6"/>
+        <v>354</v>
+      </c>
       <c r="E120" s="2" t="s">
         <v>145</v>
       </c>
       <c r="F120" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="121">
+      <c r="A121" s="3" t="n">
+        <v>96</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F121" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -5019,862 +5026,862 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1">
       <c r="A1" s="7" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="7" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="A3" s="7" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="4">
       <c r="A4" s="7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="5">
       <c r="A5" s="7" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="6">
       <c r="A6" s="7" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="7" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="8">
       <c r="A8" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="9">
       <c r="A9" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="10">
       <c r="A10" s="7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="11">
       <c r="A11" s="7" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="12">
       <c r="A12" s="7" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="13">
       <c r="A13" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="14">
       <c r="A14" s="7" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="15">
       <c r="A15" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="16">
       <c r="A16" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="17">
       <c r="A17" s="7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="18">
       <c r="A18" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19">
       <c r="A19" s="7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="20">
       <c r="A20" s="7" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="21">
       <c r="A21" s="7" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="22">
       <c r="A22" s="7" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="23">
       <c r="A23" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="24">
       <c r="A24" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="25">
       <c r="A25" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="26">
       <c r="A26" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="27">
       <c r="A27" s="7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="28">
       <c r="A28" s="7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="29">
       <c r="A29" s="7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="30">
       <c r="A30" s="7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="31">
       <c r="A31" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="32">
       <c r="A32" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="33">
       <c r="A33" s="7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="34">
       <c r="A34" s="7" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="35">
       <c r="A35" s="7" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="36">
       <c r="A36" s="7" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="37">
       <c r="A37" s="7" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="38">
       <c r="A38" s="7" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="39">
       <c r="A39" s="7" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="40">
       <c r="A40" s="7" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="41">
       <c r="A41" s="7" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="42">
       <c r="A42" s="7" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="43">
       <c r="A43" s="7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="44">
       <c r="A44" s="7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="45">
       <c r="A45" s="7" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="46">
       <c r="A46" s="7" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="47">
       <c r="A47" s="7" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="48">
       <c r="A48" s="7" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="49">
       <c r="A49" s="7" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="50">
       <c r="A50" s="7" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="51">
       <c r="A51" s="7" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="52">
       <c r="A52" s="7" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="53">
       <c r="A53" s="7" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="54">
       <c r="A54" s="7" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="55">
       <c r="A55" s="7" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="56">
       <c r="A56" s="7" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="57">
       <c r="A57" s="7" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="58">
       <c r="A58" s="7" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="60">
       <c r="A60" s="7" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="61">
       <c r="A61" s="7" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="62">
       <c r="A62" s="7" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="63">
       <c r="A63" s="7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="64">
       <c r="A64" s="7" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="65">
       <c r="A65" s="7" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="66">
       <c r="A66" s="7" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="67">
       <c r="A67" s="7" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="68">
       <c r="A68" s="7" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="69">
       <c r="A69" s="7" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="70">
       <c r="A70" s="7" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="71">
       <c r="A71" s="7" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="72">
       <c r="A72" s="7" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="73">
       <c r="A73" s="7" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="74">
       <c r="A74" s="7" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="75">
       <c r="A75" s="7" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="76">
       <c r="A76" s="7" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="77">
       <c r="A77" s="7" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="78">
       <c r="A78" s="7" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="79">
       <c r="A79" s="7" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="80">
       <c r="A80" s="7" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="81">
       <c r="A81" s="7" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="82">
       <c r="A82" s="7" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="83">
       <c r="A83" s="7" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="84">
       <c r="A84" s="7" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="85">
       <c r="A85" s="7" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="86">
       <c r="A86" s="7" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="87">
       <c r="A87" s="7" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="88">
       <c r="A88" s="7" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="89">
       <c r="A89" s="7" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="90">
       <c r="A90" s="7" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="91">
       <c r="A91" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="92">
       <c r="A92" s="7" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="93">
       <c r="A93" s="7" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="94">
       <c r="A94" s="7" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="95">
       <c r="A95" s="7" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="96">
       <c r="A96" s="7" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="97">
       <c r="A97" s="7" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="98">
       <c r="A98" s="7" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="99">
       <c r="A99" s="7" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="100">
       <c r="A100" s="7" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="101">
       <c r="A101" s="7" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="102">
       <c r="A102" s="7" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="103">
       <c r="A103" s="7" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="104">
       <c r="A104" s="7" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="105">
       <c r="A105" s="7" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="106">
       <c r="A106" s="7" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="107">
       <c r="A107" s="7" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="108">
       <c r="A108" s="7" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="109">
       <c r="A109" s="7" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="110">
       <c r="A110" s="7" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="111">
       <c r="A111" s="7" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="112">
       <c r="A112" s="7" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="113">
       <c r="A113" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="114">
       <c r="A114" s="7" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="115">
       <c r="A115" s="7" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="116">
       <c r="A116" s="7" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="117">
       <c r="A117" s="7" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="118">
       <c r="A118" s="7" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="119">
       <c r="A119" s="7" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="120">
       <c r="A120" s="7" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="121">
       <c r="A121" s="7" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="122">
       <c r="A122" s="7" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="123">
       <c r="A123" s="7" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="124">
       <c r="A124" s="7" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="125">
       <c r="A125" s="7" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="126">
       <c r="A126" s="7" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="127">
       <c r="A127" s="7" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="128">
       <c r="A128" s="7" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="129">
       <c r="A129" s="7" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="130">
       <c r="A130" s="7" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="131">
       <c r="A131" s="7" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="132">
       <c r="A132" s="7" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="133">
       <c r="A133" s="7" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="134">
       <c r="A134" s="7" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="135">
       <c r="A135" s="7" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="136">
       <c r="A136" s="7" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="137">
       <c r="A137" s="7" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="138">
       <c r="A138" s="7" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="139">
       <c r="A139" s="7" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="140">
       <c r="A140" s="7" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="141">
       <c r="A141" s="7" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="142">
       <c r="A142" s="7" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="143">
       <c r="A143" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="144">
       <c r="A144" s="7" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="145">
       <c r="A145" s="7" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="146">
       <c r="A146" s="7" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="147">
       <c r="A147" s="7" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="148">
       <c r="A148" s="7" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="149">
       <c r="A149" s="7" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="150">
       <c r="A150" s="7" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="151">
       <c r="A151" s="7" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="152">
       <c r="A152" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="153">
       <c r="A153" s="7" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="154">
       <c r="A154" s="7" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="155">
       <c r="A155" s="7" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="156">
       <c r="A156" s="7" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="157">
       <c r="A157" s="7" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="158">
       <c r="A158" s="7" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="159">
       <c r="A159" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="160">
       <c r="A160" s="7" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="161">
       <c r="A161" s="7" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="162">
       <c r="A162" s="7" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="163">
       <c r="A163" s="7" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="164">
       <c r="A164" s="7" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="165">
       <c r="A165" s="7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="166">
       <c r="A166" s="7" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="167">
       <c r="A167" s="7" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="168">
       <c r="A168" s="7" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="169">
       <c r="A169" s="7" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="170">
       <c r="A170" s="7" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="171">
       <c r="A171" s="7" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="172">
       <c r="A172" s="7" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="173">
       <c r="A173" s="7" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added LoggedElswhere message to packets and SVN :)
</commit_message>
<xml_diff>
--- a/RN and Misc/Packets.xlsx
+++ b/RN and Misc/Packets.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="527">
   <si>
     <t>Message ID</t>
   </si>
@@ -947,6 +947,9 @@
   </si>
   <si>
     <t>Server Full</t>
+  </si>
+  <si>
+    <t>97</t>
   </si>
   <si>
     <t>l3</t>
@@ -2905,8 +2908,8 @@
   </sheetPr>
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A45" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F65" activeCellId="0" pane="topLeft" sqref="F65"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A85" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C94" activeCellId="0" pane="topLeft" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4522,13 +4525,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="94">
       <c r="A94" s="6" t="s">
-        <v>67</v>
+        <v>310</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>145</v>
@@ -4542,10 +4545,10 @@
         <v>79</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>145</v>
@@ -4559,10 +4562,10 @@
         <v>80</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>145</v>
@@ -4576,10 +4579,10 @@
         <v>81</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>145</v>
@@ -4593,10 +4596,10 @@
         <v>82</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>145</v>
@@ -4610,10 +4613,10 @@
         <v>82</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>145</v>
@@ -4627,10 +4630,10 @@
         <v>82</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>145</v>
@@ -4644,10 +4647,10 @@
         <v>82</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>145</v>
@@ -4661,10 +4664,10 @@
         <v>82</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>145</v>
@@ -4715,7 +4718,7 @@
         <v>52</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>145</v>
@@ -4729,10 +4732,10 @@
         <v>86</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>145</v>
@@ -4746,7 +4749,7 @@
         <v>87</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>307</v>
@@ -4763,10 +4766,10 @@
         <v>87</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>145</v>
@@ -4780,10 +4783,10 @@
         <v>87</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>145</v>
@@ -4797,10 +4800,10 @@
         <v>87</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>145</v>
@@ -4814,10 +4817,10 @@
         <v>87</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>145</v>
@@ -4831,10 +4834,10 @@
         <v>87</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>145</v>
@@ -4848,10 +4851,10 @@
         <v>88</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>145</v>
@@ -4865,10 +4868,10 @@
         <v>89</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>145</v>
@@ -4882,10 +4885,10 @@
         <v>90</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>145</v>
@@ -4899,10 +4902,10 @@
         <v>91</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>145</v>
@@ -4916,10 +4919,10 @@
         <v>92</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>145</v>
@@ -4936,7 +4939,7 @@
         <v>67</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>145</v>
@@ -4953,7 +4956,7 @@
         <v>67</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>145</v>
@@ -4970,7 +4973,7 @@
         <v>67</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>145</v>
@@ -4987,7 +4990,7 @@
         <v>67</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>145</v>
@@ -5026,862 +5029,862 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1">
       <c r="A1" s="7" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="7" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="A3" s="7" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="4">
       <c r="A4" s="7" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="5">
       <c r="A5" s="7" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="6">
       <c r="A6" s="7" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="7" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="8">
       <c r="A8" s="7" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="9">
       <c r="A9" s="7" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="10">
       <c r="A10" s="7" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="11">
       <c r="A11" s="7" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="12">
       <c r="A12" s="7" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="13">
       <c r="A13" s="7" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="14">
       <c r="A14" s="7" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="15">
       <c r="A15" s="7" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="16">
       <c r="A16" s="7" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="17">
       <c r="A17" s="7" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="18">
       <c r="A18" s="7" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19">
       <c r="A19" s="7" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="20">
       <c r="A20" s="7" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="21">
       <c r="A21" s="7" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="22">
       <c r="A22" s="7" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="23">
       <c r="A23" s="7" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="24">
       <c r="A24" s="7" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="25">
       <c r="A25" s="7" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="26">
       <c r="A26" s="7" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="27">
       <c r="A27" s="7" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="28">
       <c r="A28" s="7" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="29">
       <c r="A29" s="7" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="30">
       <c r="A30" s="7" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="31">
       <c r="A31" s="7" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="32">
       <c r="A32" s="7" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="33">
       <c r="A33" s="7" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="34">
       <c r="A34" s="7" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="35">
       <c r="A35" s="7" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="36">
       <c r="A36" s="7" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="37">
       <c r="A37" s="7" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="38">
       <c r="A38" s="7" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="39">
       <c r="A39" s="7" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="40">
       <c r="A40" s="7" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="41">
       <c r="A41" s="7" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="42">
       <c r="A42" s="7" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="43">
       <c r="A43" s="7" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="44">
       <c r="A44" s="7" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="45">
       <c r="A45" s="7" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="46">
       <c r="A46" s="7" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="47">
       <c r="A47" s="7" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="48">
       <c r="A48" s="7" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="49">
       <c r="A49" s="7" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="50">
       <c r="A50" s="7" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="51">
       <c r="A51" s="7" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="52">
       <c r="A52" s="7" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="53">
       <c r="A53" s="7" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="54">
       <c r="A54" s="7" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="55">
       <c r="A55" s="7" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="56">
       <c r="A56" s="7" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="57">
       <c r="A57" s="7" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="58">
       <c r="A58" s="7" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="60">
       <c r="A60" s="7" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="61">
       <c r="A61" s="7" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="62">
       <c r="A62" s="7" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="63">
       <c r="A63" s="7" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="64">
       <c r="A64" s="7" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="65">
       <c r="A65" s="7" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="66">
       <c r="A66" s="7" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="67">
       <c r="A67" s="7" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="68">
       <c r="A68" s="7" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="69">
       <c r="A69" s="7" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="70">
       <c r="A70" s="7" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="71">
       <c r="A71" s="7" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="72">
       <c r="A72" s="7" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="73">
       <c r="A73" s="7" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="74">
       <c r="A74" s="7" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="75">
       <c r="A75" s="7" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="76">
       <c r="A76" s="7" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="77">
       <c r="A77" s="7" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="78">
       <c r="A78" s="7" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="79">
       <c r="A79" s="7" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="80">
       <c r="A80" s="7" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="81">
       <c r="A81" s="7" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="82">
       <c r="A82" s="7" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="83">
       <c r="A83" s="7" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="84">
       <c r="A84" s="7" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="85">
       <c r="A85" s="7" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="86">
       <c r="A86" s="7" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="87">
       <c r="A87" s="7" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="88">
       <c r="A88" s="7" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="89">
       <c r="A89" s="7" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="90">
       <c r="A90" s="7" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="91">
       <c r="A91" s="7" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="92">
       <c r="A92" s="7" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="93">
       <c r="A93" s="7" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="94">
       <c r="A94" s="7" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="95">
       <c r="A95" s="7" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="96">
       <c r="A96" s="7" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="97">
       <c r="A97" s="7" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="98">
       <c r="A98" s="7" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="99">
       <c r="A99" s="7" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="100">
       <c r="A100" s="7" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="101">
       <c r="A101" s="7" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="102">
       <c r="A102" s="7" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="103">
       <c r="A103" s="7" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="104">
       <c r="A104" s="7" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="105">
       <c r="A105" s="7" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="106">
       <c r="A106" s="7" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="107">
       <c r="A107" s="7" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="108">
       <c r="A108" s="7" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="109">
       <c r="A109" s="7" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="110">
       <c r="A110" s="7" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="111">
       <c r="A111" s="7" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="112">
       <c r="A112" s="7" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="113">
       <c r="A113" s="7" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="114">
       <c r="A114" s="7" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="115">
       <c r="A115" s="7" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="116">
       <c r="A116" s="7" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="117">
       <c r="A117" s="7" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="118">
       <c r="A118" s="7" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="119">
       <c r="A119" s="7" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="120">
       <c r="A120" s="7" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="121">
       <c r="A121" s="7" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="122">
       <c r="A122" s="7" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="123">
       <c r="A123" s="7" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="124">
       <c r="A124" s="7" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="125">
       <c r="A125" s="7" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="126">
       <c r="A126" s="7" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="127">
       <c r="A127" s="7" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="128">
       <c r="A128" s="7" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="129">
       <c r="A129" s="7" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="130">
       <c r="A130" s="7" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="131">
       <c r="A131" s="7" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="132">
       <c r="A132" s="7" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="133">
       <c r="A133" s="7" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="134">
       <c r="A134" s="7" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="135">
       <c r="A135" s="7" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="136">
       <c r="A136" s="7" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="137">
       <c r="A137" s="7" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="138">
       <c r="A138" s="7" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="139">
       <c r="A139" s="7" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="140">
       <c r="A140" s="7" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="141">
       <c r="A141" s="7" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="142">
       <c r="A142" s="7" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="143">
       <c r="A143" s="7" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="144">
       <c r="A144" s="7" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="145">
       <c r="A145" s="7" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="146">
       <c r="A146" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="147">
       <c r="A147" s="7" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="148">
       <c r="A148" s="7" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="149">
       <c r="A149" s="7" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="150">
       <c r="A150" s="7" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="151">
       <c r="A151" s="7" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="152">
       <c r="A152" s="7" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="153">
       <c r="A153" s="7" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="154">
       <c r="A154" s="7" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="155">
       <c r="A155" s="7" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="156">
       <c r="A156" s="7" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="157">
       <c r="A157" s="7" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="158">
       <c r="A158" s="7" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="159">
       <c r="A159" s="7" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="160">
       <c r="A160" s="7" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="161">
       <c r="A161" s="7" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="162">
       <c r="A162" s="7" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="163">
       <c r="A163" s="7" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="164">
       <c r="A164" s="7" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="165">
       <c r="A165" s="7" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="166">
       <c r="A166" s="7" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="167">
       <c r="A167" s="7" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="168">
       <c r="A168" s="7" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="169">
       <c r="A169" s="7" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="170">
       <c r="A170" s="7" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="171">
       <c r="A171" s="7" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="172">
       <c r="A172" s="7" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="173">
       <c r="A173" s="7" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>